<commit_message>
[PHOENIX-5860] Create Trade License Screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="tradeLocationDetails" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>dataName</t>
   </si>
@@ -23,10 +24,52 @@
     <t>aadhaarNumber</t>
   </si>
   <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>tradeOwnerName</t>
+  </si>
+  <si>
+    <t>fatherSpouseName</t>
+  </si>
+  <si>
+    <t>emailID</t>
+  </si>
+  <si>
+    <t>tradeOwnerAddress</t>
+  </si>
+  <si>
     <t>ownerDetailsTradeLicense</t>
   </si>
   <si>
     <t>11111111</t>
+  </si>
+  <si>
+    <t>Bimal</t>
+  </si>
+  <si>
+    <t>Ajaya kumar</t>
+  </si>
+  <si>
+    <t>bimal@gmail.com</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>propertyAssessmentDetails</t>
+  </si>
+  <si>
+    <t>ownershipType</t>
+  </si>
+  <si>
+    <t>locationDetailsTradeLicense</t>
+  </si>
+  <si>
+    <t>1016017647</t>
+  </si>
+  <si>
+    <t>Own</t>
   </si>
 </sst>
 </file>
@@ -61,7 +104,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,12 +170,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -152,10 +207,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -166,7 +221,8 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4795918367347"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.5561224489796"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -176,18 +232,49 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>9876798654</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="bimal@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -196,4 +283,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PHOENIX-5860] Updated Create Trade License Screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="tradeLocationDetails" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="tradeDetails" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>dataName</t>
   </si>
@@ -70,6 +71,48 @@
   </si>
   <si>
     <t>Own</t>
+  </si>
+  <si>
+    <t>tradeTitle</t>
+  </si>
+  <si>
+    <t>tradeType</t>
+  </si>
+  <si>
+    <t>tradeCategory</t>
+  </si>
+  <si>
+    <t>tradeSubCategory</t>
+  </si>
+  <si>
+    <t>tradeAreaWeightOfPremises</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>tradeCommencementDate</t>
+  </si>
+  <si>
+    <t>tradeDetailsTradeLicense</t>
+  </si>
+  <si>
+    <t>New Trade</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Flammables</t>
+  </si>
+  <si>
+    <t>Petrol or Diesel bunks</t>
+  </si>
+  <si>
+    <t>Trade Data Filled</t>
+  </si>
+  <si>
+    <t>11/12/2016</t>
   </si>
 </sst>
 </file>
@@ -153,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -188,6 +231,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -292,8 +339,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -335,4 +382,91 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="27.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PHOENIX-5860] Updated Create and search Trade License Screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
     <t>ownerDetailsTradeLicense</t>
   </si>
   <si>
-    <t>11111111</t>
+    <t>123456789123</t>
   </si>
   <si>
     <t>Bimal</t>
@@ -196,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,7 +218,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -231,10 +231,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -256,8 +252,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -391,8 +387,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -402,58 +398,58 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="27.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0867346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.780612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="8" t="s">

</xml_diff>

<commit_message>
[PHOENIX-5860] updated Collect fee trade License feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="tradeLocationDetails" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="tradeDetails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="legacyDetails" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>dataName</t>
   </si>
@@ -67,7 +68,7 @@
     <t>locationDetailsTradeLicense</t>
   </si>
   <si>
-    <t>1016017647</t>
+    <t>1016047857</t>
   </si>
   <si>
     <t>Own</t>
@@ -106,13 +107,22 @@
     <t>Flammables</t>
   </si>
   <si>
-    <t>Petrol or Diesel bunks</t>
+    <t>Acetylene Gas</t>
   </si>
   <si>
     <t>Trade Data Filled</t>
   </si>
   <si>
     <t>11/12/2016</t>
+  </si>
+  <si>
+    <t>data Name</t>
+  </si>
+  <si>
+    <t>Fee Details</t>
+  </si>
+  <si>
+    <t>legency Trade</t>
   </si>
 </sst>
 </file>
@@ -252,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -336,7 +346,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -388,7 +398,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -465,4 +475,46 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PHOENIX-5917] updated fee details in legacy Trade License
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -11,14 +11,14 @@
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="tradeLocationDetails" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="tradeDetails" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="legacyDetails" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="legencyDetails" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>dataName</t>
   </si>
@@ -116,10 +116,22 @@
     <t>11/12/2016</t>
   </si>
   <si>
-    <t>data Name</t>
-  </si>
-  <si>
-    <t>Fee Details</t>
+    <t>amount1</t>
+  </si>
+  <si>
+    <t>amountB</t>
+  </si>
+  <si>
+    <t>amountC</t>
+  </si>
+  <si>
+    <t>amountD</t>
+  </si>
+  <si>
+    <t>amountE</t>
+  </si>
+  <si>
+    <t>amountF</t>
   </si>
   <si>
     <t>legency Trade</t>
@@ -206,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +253,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -398,7 +414,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -482,30 +498,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5899] Modified the assertion statement
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,127 +14,132 @@
     <sheet name="legencyDetails" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
-    <t>dataName</t>
-  </si>
-  <si>
-    <t>aadhaarNumber</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>tradeOwnerName</t>
-  </si>
-  <si>
-    <t>fatherSpouseName</t>
-  </si>
-  <si>
-    <t>emailID</t>
-  </si>
-  <si>
-    <t>tradeOwnerAddress</t>
-  </si>
-  <si>
-    <t>ownerDetailsTradeLicense</t>
-  </si>
-  <si>
-    <t>123456789123</t>
-  </si>
-  <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Ajaya kumar</t>
-  </si>
-  <si>
-    <t>bimal@gmail.com</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>propertyAssessmentDetails</t>
-  </si>
-  <si>
-    <t>ownershipType</t>
-  </si>
-  <si>
-    <t>locationDetailsTradeLicense</t>
-  </si>
-  <si>
-    <t>1016047857</t>
-  </si>
-  <si>
-    <t>Own</t>
-  </si>
-  <si>
-    <t>tradeTitle</t>
-  </si>
-  <si>
-    <t>tradeType</t>
-  </si>
-  <si>
-    <t>tradeCategory</t>
-  </si>
-  <si>
-    <t>tradeSubCategory</t>
-  </si>
-  <si>
-    <t>tradeAreaWeightOfPremises</t>
-  </si>
-  <si>
-    <t>remarks</t>
-  </si>
-  <si>
-    <t>tradeCommencementDate</t>
-  </si>
-  <si>
-    <t>tradeDetailsTradeLicense</t>
-  </si>
-  <si>
-    <t>New Trade</t>
-  </si>
-  <si>
-    <t>Permanent</t>
-  </si>
-  <si>
-    <t>Flammables</t>
-  </si>
-  <si>
-    <t>Acetylene Gas</t>
-  </si>
-  <si>
-    <t>Trade Data Filled</t>
-  </si>
-  <si>
-    <t>11/12/2016</t>
-  </si>
-  <si>
-    <t>amount1</t>
-  </si>
-  <si>
-    <t>amountB</t>
-  </si>
-  <si>
-    <t>amountC</t>
-  </si>
-  <si>
-    <t>amountD</t>
-  </si>
-  <si>
-    <t>amountE</t>
-  </si>
-  <si>
-    <t>amountF</t>
-  </si>
-  <si>
-    <t>legency Trade</t>
+    <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aadhaarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeOwnerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fatherSpouseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeOwnerAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerDetailsTradeLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456789123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajaya kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyAssessmentDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownershipType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationDetailsTradeLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016047857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Own</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeSubCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeAreaWeightOfPremises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeCommencementDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tradeDetailsTradeLicense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Trade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permanent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flammables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetylene Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trade Data Filled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amountB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amountC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amountD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amountE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amountF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legencyTrade</t>
   </si>
 </sst>
 </file>
@@ -142,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
@@ -284,14 +289,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,7 +351,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -367,10 +372,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,7 +403,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -419,15 +424,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,7 +490,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -501,14 +506,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,7 +565,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-6076] completed Trade License Closure
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="990" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="tradeOwnerDetails" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="tradeLocationDetails" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="tradeDetails" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="legencyDetails" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="tradeLocationDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="tradeDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="legencyDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="licenseClosure" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>dataName</t>
   </si>
@@ -135,18 +135,28 @@
   </si>
   <si>
     <t>legencyTrade</t>
+  </si>
+  <si>
+    <t>licenceForClosure</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Eating Establishments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -155,25 +165,16 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,7 +186,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -193,108 +194,355 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="11.3418367346939"/>
+    <col min="1" max="1" width="19" style="1"/>
+    <col min="2" max="2" width="20.5703125" style="1"/>
+    <col min="3" max="3" width="19.28515625" style="1"/>
+    <col min="4" max="4" width="23.140625" style="1"/>
+    <col min="5" max="5" width="25.28515625" style="1"/>
+    <col min="6" max="6" width="23.7109375" style="1"/>
+    <col min="7" max="7" width="22.85546875" style="1"/>
+    <col min="8" max="1025" width="11.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -317,14 +565,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>9876798654</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -342,12 +590,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="bimal@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -355,25 +602,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col min="1" max="1" width="20.28515625"/>
+    <col min="2" max="2" width="24.5703125"/>
+    <col min="3" max="3" width="19.42578125"/>
+    <col min="4" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -384,7 +628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -396,10 +640,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -407,30 +650,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col min="1" max="1" width="25.28515625"/>
+    <col min="2" max="2" width="17.42578125"/>
+    <col min="3" max="3" width="11.28515625"/>
+    <col min="4" max="4" width="18.7109375"/>
+    <col min="5" max="5" width="18.5703125"/>
+    <col min="6" max="6" width="26.7109375"/>
+    <col min="7" max="7" width="17"/>
+    <col min="8" max="8" width="27.42578125"/>
+    <col min="9" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -456,7 +696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -472,7 +712,7 @@
       <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="7">
         <v>100</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -483,10 +723,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -494,24 +733,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="9" width="11.3418367346939"/>
+    <col min="1" max="1" width="13.7109375" style="9"/>
+    <col min="2" max="2" width="16.42578125" style="9"/>
+    <col min="3" max="1025" width="11.28515625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -534,36 +770,77 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="9">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="9">
         <v>20</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="9">
         <v>30</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="9">
         <v>40</v>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="9">
         <v>50</v>
       </c>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="9">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PHOENIX-5854] refactoring Trade License Module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="826" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>dataName</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>01/03/2017</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>ward</t>
+  </si>
+  <si>
+    <t>kotha peta</t>
+  </si>
+  <si>
+    <t>Revenue Ward No 41</t>
   </si>
 </sst>
 </file>
@@ -545,15 +557,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="1"/>
     <col min="2" max="2" width="20.5703125" style="1"/>
-    <col min="3" max="3" width="19.28515625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="1"/>
     <col min="5" max="5" width="25.28515625" style="1"/>
     <col min="6" max="6" width="23.7109375" style="1"/>
@@ -592,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>9876798654</v>
+        <v>9036544535</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -622,21 +634,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625"/>
-    <col min="2" max="2" width="24.5703125"/>
-    <col min="3" max="3" width="19.42578125"/>
-    <col min="4" max="1025" width="11.28515625"/>
+    <col min="1" max="1" width="20.28515625" style="9"/>
+    <col min="2" max="2" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="9"/>
+    <col min="6" max="1027" width="11.28515625" style="9"/>
+    <col min="1028" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -644,23 +659,35 @@
         <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -672,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[PHOENIX-5854] changes in Trade license work flow wrt PHOENIX-6335
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="826" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="826" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -861,13 +861,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>